<commit_message>
Covered else blocks and catch blocks
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/user.xlsx
+++ b/src/main/resources/excel/user.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TGS\WSpace\GitCmds\shoppingcart\src\main\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView windowHeight="3930" windowWidth="16260" xWindow="0" yWindow="0"/>
   </bookViews>
@@ -10,12 +15,11 @@
     <sheet name="User Details" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="10">
   <si>
     <t>firstName</t>
   </si>
@@ -391,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -413,7 +417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -426,16 +430,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="11">
+      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -449,7 +448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -463,7 +462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -477,7 +476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -491,7 +490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -505,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -519,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -533,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -547,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -561,7 +560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -575,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -589,7 +588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -603,7 +602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -617,7 +616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -631,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -645,7 +644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -659,7 +658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -673,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -687,7 +686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -701,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -715,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -729,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -743,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -757,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -771,7 +770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -785,7 +784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -799,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -810,6 +809,258 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>